<commit_message>
flux time change triangle
</commit_message>
<xml_diff>
--- a/SOFTWARE/Thermal/1D forloops/Layup4sensitivity.xlsx
+++ b/SOFTWARE/Thermal/1D forloops/Layup4sensitivity.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="192" yWindow="120" windowWidth="13380" windowHeight="3984"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
+    <sheet name="sensitivity flux magnitude" sheetId="1" r:id="rId1"/>
+    <sheet name="sensitivity flux duration" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -135,7 +135,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Blad1!$A$2:$A$9</c:f>
+              <c:f>'sensitivity flux magnitude'!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -168,7 +168,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$B$2:$B$9</c:f>
+              <c:f>'sensitivity flux magnitude'!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -209,11 +209,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="52971008"/>
-        <c:axId val="50199936"/>
+        <c:axId val="213860352"/>
+        <c:axId val="213862272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52971008"/>
+        <c:axId val="213860352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -248,12 +248,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50199936"/>
+        <c:crossAx val="213862272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50199936"/>
+        <c:axId val="213862272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -288,7 +288,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52971008"/>
+        <c:crossAx val="213860352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -329,16 +329,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>